<commit_message>
commiting files after pushing the weekly pagination method to base class
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite GeneralTaxRateWeek4LDOD1BRNTOTK50percentRL201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite GeneralTaxRateWeek4LDOD1BRNTOTK50percentRL201718.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="43">
   <si>
     <t>TC</t>
   </si>
@@ -796,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>